<commit_message>
Filenames amended to reflect content - MOC
</commit_message>
<xml_diff>
--- a/2020-06 Newton Hall Stock Take.xlsx
+++ b/2020-06 Newton Hall Stock Take.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Food Supply Manager\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\Foodstore-Stock-Takes\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DCF6B3-7834-477A-A1C8-7FA01BE7F898}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -74,7 +83,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -136,18 +145,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,13 +437,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:P170"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,50 +465,50 @@
     <col min="15" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="6" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2891,7 +2901,7 @@
       <c r="A79" s="1">
         <v>13.06</v>
       </c>
-      <c r="B79" s="6"/>
+      <c r="B79" s="4"/>
       <c r="C79" s="1">
         <v>14.92</v>
       </c>
@@ -4706,67 +4716,67 @@
       <c r="O170" s="1"/>
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A171" s="6">
+      <c r="A171" s="4">
         <f t="shared" ref="A171:B171" si="0">SUM(A2:A170)</f>
         <v>1547.3400000000004</v>
       </c>
-      <c r="B171" s="6">
+      <c r="B171" s="4">
         <f t="shared" si="0"/>
         <v>1056.6000000000001</v>
       </c>
-      <c r="C171" s="6">
+      <c r="C171" s="4">
         <f>SUM(C2:C153)</f>
         <v>1873.049999999999</v>
       </c>
-      <c r="D171" s="6">
+      <c r="D171" s="4">
         <f t="shared" ref="D171:O171" si="1">SUM(D2:D170)</f>
         <v>15.139999999999999</v>
       </c>
-      <c r="E171" s="6">
+      <c r="E171" s="4">
         <f t="shared" si="1"/>
         <v>6.1999999999999993</v>
       </c>
-      <c r="F171" s="6">
+      <c r="F171" s="4">
         <f t="shared" si="1"/>
         <v>383.12</v>
       </c>
-      <c r="G171" s="6">
+      <c r="G171" s="4">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="H171" s="6">
+      <c r="H171" s="4">
         <f t="shared" si="1"/>
         <v>2007.700000000001</v>
       </c>
-      <c r="I171" s="6">
+      <c r="I171" s="4">
         <f t="shared" si="1"/>
         <v>360.78</v>
       </c>
-      <c r="J171" s="6">
+      <c r="J171" s="4">
         <f t="shared" si="1"/>
         <v>422.66</v>
       </c>
-      <c r="K171" s="6">
+      <c r="K171" s="4">
         <f t="shared" si="1"/>
         <v>237.58</v>
       </c>
-      <c r="L171" s="6">
+      <c r="L171" s="4">
         <f t="shared" si="1"/>
         <v>96.399999999999977</v>
       </c>
-      <c r="M171" s="6">
+      <c r="M171" s="4">
         <f t="shared" si="1"/>
         <v>331.26</v>
       </c>
-      <c r="N171" s="6">
+      <c r="N171" s="4">
         <f t="shared" si="1"/>
         <v>461.06000000000006</v>
       </c>
-      <c r="O171" s="6">
+      <c r="O171" s="4">
         <f t="shared" si="1"/>
         <v>521.44000000000005</v>
       </c>
-      <c r="P171" s="5">
+      <c r="P171" s="3">
         <f>SUM(A171:O171)</f>
         <v>9354.33</v>
       </c>
@@ -4778,6 +4788,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C1CA48CEC719184D85A73E660997F88B" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5b62705be076f6b8499c49472fd1fe9f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="175bd3b9-7edf-4a4a-b9d1-7186fb46ae82" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7080b9af62254c11f73159494d1ae1d3" ns2:_="">
     <xsd:import namespace="175bd3b9-7edf-4a4a-b9d1-7186fb46ae82"/>
@@ -4955,29 +4980,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE4B7D7-9933-487B-9721-6FFBE691B4D6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F21ECDA-6089-4A73-A190-AF086470634D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1921D5-12C1-4591-B6A2-34631E8C582C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A1921D5-12C1-4591-B6A2-34631E8C582C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F21ECDA-6089-4A73-A190-AF086470634D}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DE4B7D7-9933-487B-9721-6FFBE691B4D6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="175bd3b9-7edf-4a4a-b9d1-7186fb46ae82"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>